<commit_message>
correciones foto modelo anemico citareserva y pagos
</commit_message>
<xml_diff>
--- a/SpaOnline/ModeloDominio/CitaReserva - Muestreo Datos.xlsx
+++ b/SpaOnline/ModeloDominio/CitaReserva - Muestreo Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOO\DOO\SpaOnline\ModeloDominio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis ospina\OneDrive\Documentos\GitHub\DOO\SpaOnline\ModeloDominio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72DE751-9E38-4955-8AA1-23F821C66D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039ADD6F-D6FF-4573-B75B-F7C4F80F6459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="2" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de Dominio Anemico" sheetId="1" r:id="rId1"/>
@@ -416,20 +416,20 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>20329</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>556</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>39169</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114927</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BED785A-023C-FD26-F2EE-00978BCC7A85}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A02D6240-A0DA-A164-F339-511E4235C3C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -445,8 +445,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="19050"/>
-          <a:ext cx="9164329" cy="3982006"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7659169" cy="4496427"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA198BEE-AB41-4447-8B76-5672FB9C01F4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,7 +937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE5137F-269A-4BBF-8793-E8FCF1AB8F55}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1142,7 +1142,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>